<commit_message>
Fixat sortering i Ritningssortering
</commit_message>
<xml_diff>
--- a/Tidsredovinsing/AMEK Tidsredovisning 2019-2021.xlsx
+++ b/Tidsredovinsing/AMEK Tidsredovisning 2019-2021.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F00FA3-63D5-4E19-B4F6-47CD75A4C9F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADED559E-382E-4851-9F00-8A294EE7F431}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="810" windowWidth="23385" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="465" windowWidth="23385" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Datum</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Hantering av ritningsnotiser i Ordus och ordusrapport, test och deploy</t>
+  </si>
+  <si>
+    <t>Ändra, utskrift, sortering , visa av ritningsnotiser</t>
+  </si>
+  <si>
+    <t>Extra visning av ritningsnotering i Orderfönstret</t>
   </si>
 </sst>
 </file>
@@ -600,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G46"/>
+  <dimension ref="A2:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,6 +1203,28 @@
         <v>42</v>
       </c>
     </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>43921</v>
+      </c>
+      <c r="B47" s="9">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>43925</v>
+      </c>
+      <c r="B48" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:C24">
     <sortCondition ref="A4"/>

</xml_diff>